<commit_message>
Major restructuring and cleanup
</commit_message>
<xml_diff>
--- a/Writings/Data Dimensions.xlsx
+++ b/Writings/Data Dimensions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aaudk-my.sharepoint.com/personal/sf51ki_id_aau_dk/Documents/Dokumenter/Kaggle Project/kaggle-project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SF51KI\OneDrive - Aalborg Universitet\Dokumenter\Kaggle Project\kaggle-project\Writings\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t xml:space="preserve">Competition </t>
   </si>
@@ -108,12 +108,6 @@
   </si>
   <si>
     <t># Seasons</t>
-  </si>
-  <si>
-    <t># Events</t>
-  </si>
-  <si>
-    <t>Event (Promotion)</t>
   </si>
 </sst>
 </file>
@@ -122,8 +116,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="171" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="172" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -262,11 +256,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Komma" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -283,9 +277,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Kontor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -323,7 +317,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kontor">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -395,7 +389,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kontor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -548,7 +542,7 @@
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -591,12 +585,8 @@
       <c r="J1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="K1" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>28</v>
-      </c>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
     </row>
     <row r="2" spans="1:12" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
@@ -815,6 +805,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100CFAC39541BC0884988008E23BCB17235" ma:contentTypeVersion="10" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="afcf8bf3e4c307d1083d70ef0d579815">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8fe2c115-ee5e-4abc-863d-b44282071455" xmlns:ns4="7fe73e4e-19b4-4f1f-9a2b-d8e50d92a6c3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e694b4b41272ad0fe95d374b5ec3c831" ns3:_="" ns4:_="">
     <xsd:import namespace="8fe2c115-ee5e-4abc-863d-b44282071455"/>
@@ -1017,15 +1016,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1033,6 +1023,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C759552-18E2-48CC-8953-FE90ED9C6770}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EAB4D937-0EFE-4B7E-8CBA-D7DAE9EF5E7C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1051,27 +1049,19 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C759552-18E2-48CC-8953-FE90ED9C6770}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8FCFA92-9013-4BA8-928E-7E5BAE629DDD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="7fe73e4e-19b4-4f1f-9a2b-d8e50d92a6c3"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="7fe73e4e-19b4-4f1f-9a2b-d8e50d92a6c3"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="8fe2c115-ee5e-4abc-863d-b44282071455"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>